<commit_message>
multiple bidding and natural gas
</commit_message>
<xml_diff>
--- a/Agents.xlsx
+++ b/Agents.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emirsener/Desktop/2024 Fall/IE492-Electricity-Markets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CCABEA4-BFCC-2A43-BA2F-4D6F4C32BDE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B9741FD-625E-744D-B5D5-51F0737F5F68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" xr2:uid="{02AB118A-9D15-3445-9FA1-39510F6F8703}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" activeTab="1" xr2:uid="{02AB118A-9D15-3445-9FA1-39510F6F8703}"/>
   </bookViews>
   <sheets>
     <sheet name="Sim1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="13">
   <si>
     <t>type</t>
   </si>
@@ -49,12 +49,6 @@
   </si>
   <si>
     <t>strategy_params</t>
-  </si>
-  <si>
-    <t>startup_cost</t>
-  </si>
-  <si>
-    <t>variable_cost</t>
   </si>
   <si>
     <t>producer</t>
@@ -460,21 +454,19 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B42FD3CF-19C6-F548-A839-0BECF398380C}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView zoomScale="125" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="26.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -487,65 +479,47 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
         <v>11</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2">
-        <v>50</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3">
-        <v>30</v>
-      </c>
-      <c r="F3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -557,21 +531,19 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0342D20B-BF07-4C4D-B682-A0A381C5E06C}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="26.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -584,45 +556,33 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
         <v>11</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2">
-        <v>50</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
web scrapping, adjusted structure
</commit_message>
<xml_diff>
--- a/Agents.xlsx
+++ b/Agents.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emirsener/Desktop/2024 Fall/IE492-Electricity-Markets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B9741FD-625E-744D-B5D5-51F0737F5F68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32AC428A-C215-1443-9760-93232CE9362B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" activeTab="1" xr2:uid="{02AB118A-9D15-3445-9FA1-39510F6F8703}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" xr2:uid="{02AB118A-9D15-3445-9FA1-39510F6F8703}"/>
   </bookViews>
   <sheets>
     <sheet name="Sim1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sim2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
   <si>
     <t>type</t>
   </si>
@@ -57,25 +56,37 @@
     <t>consumer</t>
   </si>
   <si>
-    <t>Coal1</t>
-  </si>
-  <si>
-    <t>Gas1</t>
-  </si>
-  <si>
-    <t>Consumer1</t>
-  </si>
-  <si>
-    <t>NaiveBiddingStrategy</t>
-  </si>
-  <si>
-    <t>MovingAverageBiddingStrategy</t>
-  </si>
-  <si>
-    <t>{'period':24}</t>
-  </si>
-  <si>
-    <t>{'window_size':3,'period':24}</t>
+    <t>{}</t>
+  </si>
+  <si>
+    <t>GasPlant1</t>
+  </si>
+  <si>
+    <t>CoalPlant1</t>
+  </si>
+  <si>
+    <t>HydroPlant1</t>
+  </si>
+  <si>
+    <t>ZeroBidders1</t>
+  </si>
+  <si>
+    <t>Consumer</t>
+  </si>
+  <si>
+    <t>NaturalGasBiddingStrategy</t>
+  </si>
+  <si>
+    <t>CoalBiddingStrategy</t>
+  </si>
+  <si>
+    <t>DammedHydroBiddingStrategy</t>
+  </si>
+  <si>
+    <t>ZeroBiddingStrategy</t>
+  </si>
+  <si>
+    <t>ConsumerBiddingStrategy</t>
   </si>
 </sst>
 </file>
@@ -454,14 +465,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B42FD3CF-19C6-F548-A839-0BECF398380C}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:G1048576"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.6640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -485,13 +497,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
         <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -499,93 +511,59 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="B6" t="s">
         <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0342D20B-BF07-4C4D-B682-A0A381C5E06C}">
-  <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:D3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="3" max="3" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.6640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>